<commit_message>
update to working state
</commit_message>
<xml_diff>
--- a/src/main/workbooks/july2025.xlsx
+++ b/src/main/workbooks/july2025.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachcraven/repos/InformationSenderApp/src/main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachcraven/repos/InformationSenderApp/src/main/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDF83703-C405-6146-979C-78C59910F6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB5BC1C-99A3-1D43-887E-E39A04802FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{7FDD2D68-E146-8C4D-A958-0FA4B21D36F3}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="2" xr2:uid="{7FDD2D68-E146-8C4D-A958-0FA4B21D36F3}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
     <sheet name="budget" sheetId="2" r:id="rId2"/>
+    <sheet name="income" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Purchase</t>
   </si>
@@ -51,9 +52,6 @@
     <t>car</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>Allocated</t>
   </si>
   <si>
@@ -64,6 +62,12 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>job2</t>
+  </si>
+  <si>
+    <t>job1</t>
   </si>
 </sst>
 </file>
@@ -439,7 +443,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -469,7 +473,7 @@
         <v>45848</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>90</v>
@@ -484,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3AB87B-3F38-1541-9632-50BE1C7795F6}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -495,21 +499,57 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2">
         <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9789E8A1-1B19-7B46-93C5-87EBF870D9C0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update email formatting / add rounding error fix
# Conflicts:
#	src/main/workbooks/july2025.xlsx
</commit_message>
<xml_diff>
--- a/src/main/workbooks/july2025.xlsx
+++ b/src/main/workbooks/july2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachcraven/repos/InformationSenderApp/src/main/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AD3915-CAC6-CC46-815E-4A03877D61F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAD5CB3-FE27-AF4B-B04D-07A2727A1990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="500" windowWidth="15240" windowHeight="16260" activeTab="1" xr2:uid="{7FDD2D68-E146-8C4D-A958-0FA4B21D36F3}"/>
+    <workbookView xWindow="13560" yWindow="500" windowWidth="15240" windowHeight="16260" xr2:uid="{7FDD2D68-E146-8C4D-A958-0FA4B21D36F3}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Winco</t>
   </si>
   <si>
-    <t>Dori</t>
-  </si>
-  <si>
     <t>Gas Station</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Cooler</t>
+  </si>
+  <si>
+    <t>Allowance</t>
   </si>
 </sst>
 </file>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE86BE8-14AF-704F-87A7-B2263C9D4C9D}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="184" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -579,11 +579,11 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -627,11 +627,11 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>14.36</v>
@@ -651,11 +651,11 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>17.899999999999999</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
@@ -711,11 +711,11 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>10.8</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
       </c>
       <c r="D18">
         <v>108.95</v>
@@ -772,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>63.76</v>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3AB87B-3F38-1541-9632-50BE1C7795F6}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+    <sheetView zoomScale="141" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>